<commit_message>
Inserção da plhanilha de risco e modificações no Backlog
</commit_message>
<xml_diff>
--- a/Documentação/(NOVO) Backlog.xlsx
+++ b/Documentação/(NOVO) Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -195,63 +195,6 @@
     <t>locais estratégicos para a melhor captação de fluxo de pessoas.</t>
   </si>
   <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>R28</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>R32</t>
-  </si>
-  <si>
-    <t>R33</t>
-  </si>
-  <si>
-    <t>R34</t>
-  </si>
-  <si>
-    <t>R35</t>
-  </si>
-  <si>
-    <t>R36</t>
-  </si>
-  <si>
-    <t>R37</t>
-  </si>
-  <si>
-    <t>R38</t>
-  </si>
-  <si>
-    <t>R39</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>RF15.1</t>
-  </si>
-  <si>
-    <t>RF17</t>
-  </si>
-  <si>
     <t>RNF17</t>
   </si>
   <si>
@@ -261,7 +204,10 @@
     <t>RNF21</t>
   </si>
   <si>
-    <t>R22</t>
+    <t>RF9</t>
+  </si>
+  <si>
+    <t>RF13.1</t>
   </si>
 </sst>
 </file>
@@ -279,53 +225,63 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -439,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -588,6 +544,28 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -690,33 +668,33 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,527 +910,491 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1005"/>
+  <dimension ref="B2:H1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="90.75" customWidth="1"/>
-    <col min="3" max="3" width="11.875" customWidth="1"/>
-    <col min="4" max="4" width="10.125" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
-    <col min="6" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="16.75" customWidth="1"/>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="98.625" customWidth="1"/>
+    <col min="4" max="4" width="11.875" customWidth="1"/>
+    <col min="5" max="5" width="10.125" customWidth="1"/>
+    <col min="6" max="6" width="7.625" customWidth="1"/>
+    <col min="7" max="7" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+    <row r="2" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="C3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="D3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="12" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="12" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23" t="s">
+      <c r="D8" s="15"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="C9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="19" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="12" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="19" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+    <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="C11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="19" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="H11" s="26"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="19" t="s">
+      <c r="D12" s="27"/>
+      <c r="E12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="12" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="19" t="s">
+      <c r="C14" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="31"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="34"/>
+      <c r="H15" s="33"/>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="35"/>
+      <c r="G16" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="36"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="39"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="42"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="42"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="41">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="47"/>
+      <c r="H22" s="41"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="61" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="34"/>
-      <c r="G13" s="33"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="35"/>
-      <c r="F14" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="62" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="36"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="39"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="42"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="41">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="42"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="41">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="62" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="41">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="47"/>
-      <c r="G20" s="41"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="50" t="s">
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="52"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="53"/>
+    </row>
+    <row r="26" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="54"/>
+    </row>
+    <row r="27" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="52"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="62" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="53"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="54"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="58"/>
-      <c r="B26" s="66" t="s">
+    <row r="28" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="66"/>
+      <c r="C28" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="56"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="56"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="56"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+    </row>
+    <row r="29" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="68"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+    </row>
+    <row r="30" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="69"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+    </row>
+    <row r="31" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="69"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+    </row>
+    <row r="32" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="65"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="65"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="69"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+    </row>
+    <row r="35" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="69"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="69"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="69"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="69"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="69"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+    </row>
+    <row r="40" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="69"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="69"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="69"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="69"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+    </row>
+    <row r="44" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="69"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="69"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+    </row>
+    <row r="46" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="69"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+    </row>
+    <row r="47" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2410,11 +2352,13 @@
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="1.8859537719075441" bottom="7.8738569977139967" header="0" footer="0"/>
   <pageSetup paperSize="8" orientation="portrait"/>

</xml_diff>

<commit_message>
Alterações no Backlog e inserção da imagem do Backlog na pasta documentos
</commit_message>
<xml_diff>
--- a/Documentação/(NOVO) Backlog.xlsx
+++ b/Documentação/(NOVO) Backlog.xlsx
@@ -174,15 +174,9 @@
     <t>O usuário do site será o funcionário escolhido pela empresa do Metrô.</t>
   </si>
   <si>
-    <t>R19</t>
-  </si>
-  <si>
     <t>O banco de dados deverá conter as tabelas :  Sensor, LinhaEstação, Linha, Estação, Usuário, Relatório.</t>
   </si>
   <si>
-    <t>R20</t>
-  </si>
-  <si>
     <t>O banco de dados deverá receber todos os dados obtidos pelo sensor  durante todo o dia.</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
     <t>RNF17</t>
   </si>
   <si>
-    <t>R18</t>
-  </si>
-  <si>
     <t>RNF21</t>
   </si>
   <si>
@@ -208,6 +199,15 @@
   </si>
   <si>
     <t>RF13.1</t>
+  </si>
+  <si>
+    <t>RF18</t>
+  </si>
+  <si>
+    <t>RF19</t>
+  </si>
+  <si>
+    <t>RF20</t>
   </si>
 </sst>
 </file>
@@ -523,17 +523,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -568,11 +557,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -623,9 +627,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -642,9 +643,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -669,7 +667,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -680,21 +677,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,7 +916,7 @@
   <dimension ref="B2:H1007"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -930,13 +933,13 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="57" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -1089,7 +1092,7 @@
     </row>
     <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>31</v>
@@ -1114,7 +1117,7 @@
       <c r="D14" s="18"/>
       <c r="E14" s="31"/>
       <c r="G14" s="32"/>
-      <c r="H14" s="55" t="s">
+      <c r="H14" s="53" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1126,7 +1129,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="18"/>
-      <c r="E15" s="34"/>
+      <c r="E15" s="67"/>
       <c r="H15" s="33"/>
     </row>
     <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1137,7 +1140,7 @@
         <v>38</v>
       </c>
       <c r="D16" s="18"/>
-      <c r="E16" s="35"/>
+      <c r="E16" s="34"/>
       <c r="G16" s="11" t="s">
         <v>3</v>
       </c>
@@ -1150,23 +1153,23 @@
         <v>40</v>
       </c>
       <c r="D17" s="24"/>
-      <c r="E17" s="36"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="38">
+      <c r="E17" s="35"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="24"/>
-      <c r="E18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41">
+      <c r="E18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40">
         <v>5</v>
       </c>
     </row>
@@ -1178,9 +1181,9 @@
         <v>43</v>
       </c>
       <c r="D19" s="15"/>
-      <c r="E19" s="42"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="41">
+      <c r="E19" s="68"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="40">
         <v>8</v>
       </c>
     </row>
@@ -1192,9 +1195,9 @@
         <v>45</v>
       </c>
       <c r="D20" s="27"/>
-      <c r="E20" s="42"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="41">
+      <c r="E20" s="68"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="40">
         <v>13</v>
       </c>
     </row>
@@ -1202,13 +1205,13 @@
       <c r="B21" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="46"/>
-      <c r="E21" s="47"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="41">
+      <c r="D21" s="44"/>
+      <c r="E21" s="45"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="40">
         <v>21</v>
       </c>
     </row>
@@ -1216,182 +1219,182 @@
       <c r="B22" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="43" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="24"/>
-      <c r="E22" s="47"/>
-      <c r="H22" s="41"/>
+      <c r="E22" s="45"/>
+      <c r="H22" s="40"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="49"/>
-      <c r="E23" s="50" t="s">
+      <c r="D23" s="47"/>
+      <c r="E23" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="51" t="s">
+      <c r="B24" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="50"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="52"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="51" t="s">
+      <c r="D25" s="15"/>
+      <c r="E25" s="51"/>
+    </row>
+    <row r="26" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="52"/>
+    </row>
+    <row r="27" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="53"/>
-    </row>
-    <row r="26" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="51" t="s">
+      <c r="D27" s="65"/>
+      <c r="E27" s="66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="64"/>
+      <c r="C28" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="54"/>
-    </row>
-    <row r="27" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="61" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="62"/>
-      <c r="E27" s="63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="66"/>
-      <c r="C28" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
     </row>
     <row r="29" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="68"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
     </row>
     <row r="30" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="69"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
     </row>
     <row r="31" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="69"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
     </row>
     <row r="32" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="65"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
     </row>
     <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="65"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
     </row>
     <row r="34" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="69"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
     </row>
     <row r="35" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="69"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
     </row>
     <row r="36" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="69"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
     </row>
     <row r="37" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="69"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
     </row>
     <row r="38" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="69"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
     </row>
     <row r="39" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="69"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
     </row>
     <row r="40" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="69"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
     </row>
     <row r="41" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="69"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
     </row>
     <row r="42" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="69"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
     </row>
     <row r="43" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="69"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
     </row>
     <row r="44" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="69"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="58"/>
     </row>
     <row r="45" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="69"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="58"/>
     </row>
     <row r="46" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="69"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
     </row>
     <row r="47" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>